<commit_message>
Began Dispatcher work, to download input data for process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239746C5-B705-449B-8F80-5DEDAF3D7E3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4007FEC-F060-4CF9-9BF5-416155DCD85A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2004" yWindow="756" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>Sheet name in workbook to read from, to demonstrate purpose of Dispatcher.xaml.</t>
+  </si>
+  <si>
+    <t>SheetKey</t>
+  </si>
+  <si>
+    <t>GSuiteAPIKey</t>
+  </si>
+  <si>
+    <t>GSuiteAPIKeyPath</t>
+  </si>
+  <si>
+    <t>Data/APIKey.txt</t>
   </si>
 </sst>
 </file>
@@ -533,7 +545,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -625,7 +637,14 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2757,7 +2776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2801,7 +2822,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated column names of response file to be Username
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4007FEC-F060-4CF9-9BF5-416155DCD85A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDDF28A-4163-4FF7-AE04-FAB2E094782B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="756" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -155,18 +155,6 @@
   </si>
   <si>
     <t>Sheet name in workbook to read from, to demonstrate purpose of Dispatcher.xaml.</t>
-  </si>
-  <si>
-    <t>SheetKey</t>
-  </si>
-  <si>
-    <t>GSuiteAPIKey</t>
-  </si>
-  <si>
-    <t>GSuiteAPIKeyPath</t>
-  </si>
-  <si>
-    <t>Data/APIKey.txt</t>
   </si>
 </sst>
 </file>
@@ -544,16 +532,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -602,7 +590,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -637,14 +625,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,12 +1629,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1690,7 +1671,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2776,16 +2757,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2822,14 +2803,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
moved over google sign in workflows from automation 1, augmented them to work with automation 2, and all this was done on the old dispatcher sequence. These changes need to be integrated into the new disatcher JJ made
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CA01E2-F761-4E54-9CF4-2655AE9371E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F4F94-8F16-40D7-B55C-DCE7B6926530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>GithubCredential</t>
+  </si>
+  <si>
+    <t>GoogleCredential</t>
+  </si>
+  <si>
+    <t>Credential for signing into the users Google account</t>
+  </si>
+  <si>
+    <t>Credential for signing into the users GitHub account</t>
   </si>
 </sst>
 </file>
@@ -535,16 +544,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.578125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.41796875" customWidth="1"/>
+    <col min="4" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -593,7 +602,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -635,8 +644,21 @@
       <c r="B9" t="s">
         <v>43</v>
       </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1635,16 +1657,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.26171875" customWidth="1"/>
+    <col min="4" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1703,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2771,12 +2793,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.68359375" customWidth="1"/>
+    <col min="2" max="2" width="30.26171875" customWidth="1"/>
+    <col min="3" max="3" width="60.26171875" customWidth="1"/>
+    <col min="4" max="26" width="65.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated Dispatcher to take in form if available
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\uipath-automation-2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F4F94-8F16-40D7-B55C-DCE7B6926530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C52961-5AB3-447E-81B0-9C33E5E81597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>Credential for signing into the users GitHub account</t>
+  </si>
+  <si>
+    <t>InputFileRelativePath</t>
+  </si>
+  <si>
+    <t>\Documents\RevatureAutomationFiles\BatchOrganizationInput.txt</t>
+  </si>
+  <si>
+    <t>The filepath used to get the input data from the user's account. This string gets added to C:\Users\&lt;UserName&gt;</t>
   </si>
 </sst>
 </file>
@@ -545,15 +554,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.578125" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -602,7 +611,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -660,7 +669,17 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1661,12 +1680,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.26171875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1703,7 +1722,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2793,12 +2812,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.68359375" customWidth="1"/>
-    <col min="2" max="2" width="30.26171875" customWidth="1"/>
-    <col min="3" max="3" width="60.26171875" customWidth="1"/>
-    <col min="4" max="26" width="65.41796875" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Writes file with JSON data if form input manually
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C52961-5AB3-447E-81B0-9C33E5E81597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D8915E-CC2A-42F7-8F91-C88321D18281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>The filepath used to get the input data from the user's account. This string gets added to C:\Users\&lt;UserName&gt;</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>BatchOrganizationInput.txt</t>
+  </si>
+  <si>
+    <t>The name of the file created when filling out the form in the GetForm component</t>
   </si>
 </sst>
 </file>
@@ -554,7 +563,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -680,7 +689,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Implemented output workflows to write transaction report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D8915E-CC2A-42F7-8F91-C88321D18281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA77C2D-55F8-4DCC-B8BF-0E588F8EDBDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>ProcessABCQueue</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>The name of the file created when filling out the form in the GetForm component</t>
+  </si>
+  <si>
+    <t>BatchGitHubOrgCreation</t>
   </si>
 </sst>
 </file>
@@ -563,15 +563,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -610,94 +610,94 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1699,12 +1699,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1741,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1773,7 +1773,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1795,7 +1795,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1806,7 +1806,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1817,30 +1817,30 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2831,12 +2831,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated filepath for input file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA77C2D-55F8-4DCC-B8BF-0E588F8EDBDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E99D71B-6EDA-4689-9EF4-B245E4517B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="5580" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>InputFileRelativePath</t>
   </si>
   <si>
-    <t>\Documents\RevatureAutomationFiles\BatchOrganizationInput.txt</t>
-  </si>
-  <si>
     <t>The filepath used to get the input data from the user's account. This string gets added to C:\Users\&lt;UserName&gt;</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>BatchGitHubOrgCreation</t>
+  </si>
+  <si>
+    <t>\RevatureAutomationFiles\</t>
   </si>
 </sst>
 </file>
@@ -563,15 +563,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -620,12 +620,12 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>23</v>
@@ -683,21 +683,21 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
         <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1699,12 +1699,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1741,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2831,12 +2831,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>